<commit_message>
update read connections example excel
</commit_message>
<xml_diff>
--- a/Examples/Dictionary/Input/ExpN_readconnections_Excel.xlsx
+++ b/Examples/Dictionary/Input/ExpN_readconnections_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/GITHUB/AhpAnpLib/Examples/Dictionary/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02DEF4F-F34F-2E45-9C08-5B039A491ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D427151-53FD-2842-B472-97A3E9465E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38240" yWindow="7220" windowWidth="38400" windowHeight="21140" xr2:uid="{85FBE8EF-A2A3-FF4A-A4E5-6C5A2BBF521C}"/>
+    <workbookView xWindow="28800" yWindow="-960" windowWidth="38400" windowHeight="21140" xr2:uid="{85FBE8EF-A2A3-FF4A-A4E5-6C5A2BBF521C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Cl1</t>
-  </si>
-  <si>
-    <t>Node1</t>
   </si>
   <si>
     <t>Cl2</t>
@@ -429,74 +426,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0AEF4B2-F327-6A4B-8567-F34D23BB6230}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
       </c>
       <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" t="s">
-        <v>13</v>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -527,9 +554,6 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -705,29 +729,32 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -740,9 +767,6 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -809,41 +833,6 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
         <v>0</v>
       </c>
     </row>

</xml_diff>